<commit_message>
3.3.1 files from US
</commit_message>
<xml_diff>
--- a/InputData/elec/BGDPbES/BAU Guaranteed Dispatch Perc by Elec Source.xlsx
+++ b/InputData/elec/BGDPbES/BAU Guaranteed Dispatch Perc by Elec Source.xlsx
@@ -1,21 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipI\InputData\elec\BGDPbES\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rorvis\Dropbox (Energy InNovation)\My Documents\Energy Policy Solutions\US\Models\eps-us-analysis\InputData\elec\BGDPbES\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{257288C8-88AB-4482-B0B3-D67DC1B2D04F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="22995" windowHeight="11055"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="BGDPbES" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -103,7 +115,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -243,6 +255,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -278,6 +307,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -453,10 +499,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -512,13 +560,15 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:AK17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1236,147 +1286,147 @@
         <v>20</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
@@ -1384,147 +1434,147 @@
         <v>3</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
@@ -1532,147 +1582,147 @@
         <v>4</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
@@ -1680,147 +1730,147 @@
         <v>5</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ9">
         <f t="shared" ref="D9:AK14" si="2">$B9</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK9">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
@@ -1828,147 +1878,147 @@
         <v>7</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK10">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
@@ -2420,147 +2470,147 @@
         <v>21</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14">
         <f>$B14</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.25">
@@ -2794,112 +2844,147 @@
         <v>24</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17">
-        <v>0</v>
+        <f>B17</f>
+        <v>1</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <f t="shared" ref="D17:AK17" si="3">C17</f>
+        <v>1</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="F17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="G17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="H17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="I17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="J17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="K17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="L17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="M17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="N17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="O17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="P17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="Q17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="R17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="S17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="T17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="U17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="V17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="W17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="X17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="Y17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="Z17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="AA17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="AB17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="AC17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="AD17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="AE17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="AF17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="AG17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="AH17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="AI17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="AJ17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="AK17">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>